<commit_message>
Fixed Timer 2 anad updated Unit test protocol sheet
</commit_message>
<xml_diff>
--- a/air conditioning/Unit Test Protocol (Air Conditioning).xlsx
+++ b/air conditioning/Unit Test Protocol (Air Conditioning).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7590"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20430" windowHeight="7275"/>
   </bookViews>
   <sheets>
     <sheet name="Unit Tests (Air Conditioning)" sheetId="1" r:id="rId1"/>
@@ -93,9 +93,6 @@
     <t>LCD Driver</t>
   </si>
   <si>
-    <t>Mohab/Omar</t>
-  </si>
-  <si>
     <t>ADC Driver</t>
   </si>
   <si>
@@ -120,21 +117,12 @@
     <t>Call TIMER2_delay(3000) to delay the code for 3 seconds</t>
   </si>
   <si>
-    <t>Call LCD_sendChar('A'),Call LCD_sendInteger(50)</t>
-  </si>
-  <si>
     <t>Buzzer should turn on</t>
   </si>
   <si>
     <t>Buzzer turned on</t>
   </si>
   <si>
-    <t xml:space="preserve">LCD should print -&gt; A50 </t>
-  </si>
-  <si>
-    <t>LCD printed A50</t>
-  </si>
-  <si>
     <t>Reading is changing according to the potetiometer position</t>
   </si>
   <si>
@@ -142,6 +130,18 @@
   </si>
   <si>
     <t>LCD is showing the pressed keys</t>
+  </si>
+  <si>
+    <t>LCD should print -&gt; a b c d and so on</t>
+  </si>
+  <si>
+    <t>Call LCD_sendChar('a') and increment it,Test Upper, lower nibble &amp; 8 bit mode by adjusting config file</t>
+  </si>
+  <si>
+    <t>LCD printed the expected values</t>
+  </si>
+  <si>
+    <t>Omar</t>
   </si>
 </sst>
 </file>
@@ -493,7 +493,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +501,7 @@
     <col min="1" max="1" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="105.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="115.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="54.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="36.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.5703125" style="3" bestFit="1" customWidth="1"/>
@@ -544,7 +544,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>15</v>
@@ -567,7 +567,7 @@
         <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>17</v>
@@ -590,7 +590,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>17</v>
@@ -613,13 +613,13 @@
         <v>4</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>13</v>
@@ -633,16 +633,16 @@
         <v>21</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>13</v>
@@ -653,19 +653,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>13</v>
@@ -676,19 +676,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>13</v>

</xml_diff>